<commit_message>
OLB-19 chore: prod cors 설정, docs 제한
</commit_message>
<xml_diff>
--- a/etc/file/korea_stock_list.xlsx
+++ b/etc/file/korea_stock_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="348">
   <si>
     <t>Symbol</t>
   </si>
@@ -372,7 +372,7 @@
     <t>001740</t>
   </si>
   <si>
-    <t>종근당</t>
+    <t>SK네트웍스</t>
   </si>
   <si>
     <t>Chong Kun Dang</t>
@@ -399,7 +399,7 @@
     <t>001800</t>
   </si>
   <si>
-    <t>삼성증권</t>
+    <t>오리온홀딩스</t>
   </si>
   <si>
     <t>Samsung Securities</t>
@@ -417,7 +417,7 @@
     <t>005830</t>
   </si>
   <si>
-    <t>동부건설</t>
+    <t>DB손해보험</t>
   </si>
   <si>
     <t>Dongbu Construction</t>
@@ -435,7 +435,7 @@
     <t>009470</t>
   </si>
   <si>
-    <t>한화솔루션</t>
+    <t>삼화전기</t>
   </si>
   <si>
     <t>Hanwha Solutions</t>
@@ -471,7 +471,7 @@
     <t>071950</t>
   </si>
   <si>
-    <t>이마트</t>
+    <t>코아스</t>
   </si>
   <si>
     <t>Emart</t>
@@ -525,97 +525,100 @@
     <t>210980</t>
   </si>
   <si>
+    <t>SK디앤디</t>
+  </si>
+  <si>
+    <t>Pearl Abyss</t>
+  </si>
+  <si>
+    <t>108320</t>
+  </si>
+  <si>
+    <t>LX세미콘</t>
+  </si>
+  <si>
+    <t>LG Innotek</t>
+  </si>
+  <si>
+    <t>한국전력공사</t>
+  </si>
+  <si>
+    <t>KEPCO</t>
+  </si>
+  <si>
+    <t>005935</t>
+  </si>
+  <si>
+    <t>삼성전자우</t>
+  </si>
+  <si>
+    <t>Samsung Electronics (Preferred)</t>
+  </si>
+  <si>
+    <t>Shinhan Financial Group</t>
+  </si>
+  <si>
+    <t>024110</t>
+  </si>
+  <si>
+    <t>기업은행</t>
+  </si>
+  <si>
+    <t>Industrial Bank of Korea</t>
+  </si>
+  <si>
+    <t>323410</t>
+  </si>
+  <si>
+    <t>카카오뱅크</t>
+  </si>
+  <si>
+    <t>KakaoBank</t>
+  </si>
+  <si>
+    <t>316140</t>
+  </si>
+  <si>
+    <t>우리금융지주</t>
+  </si>
+  <si>
+    <t>Woori Financial Group</t>
+  </si>
+  <si>
+    <t>112040</t>
+  </si>
+  <si>
+    <t>위메이드</t>
+  </si>
+  <si>
+    <t>Wemade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KOSDAQ</t>
+  </si>
+  <si>
+    <t>067160</t>
+  </si>
+  <si>
+    <t>소프트캠프</t>
+  </si>
+  <si>
+    <t>Softcamp</t>
+  </si>
+  <si>
+    <t>225570</t>
+  </si>
+  <si>
+    <t>넥슨게임즈</t>
+  </si>
+  <si>
+    <t>Nexon Games</t>
+  </si>
+  <si>
+    <t>263750</t>
+  </si>
+  <si>
     <t>펄어비스</t>
-  </si>
-  <si>
-    <t>Pearl Abyss</t>
-  </si>
-  <si>
-    <t>108320</t>
-  </si>
-  <si>
-    <t>LG이노텍</t>
-  </si>
-  <si>
-    <t>LG Innotek</t>
-  </si>
-  <si>
-    <t>한국전력공사</t>
-  </si>
-  <si>
-    <t>KEPCO</t>
-  </si>
-  <si>
-    <t>005935</t>
-  </si>
-  <si>
-    <t>삼성전자우</t>
-  </si>
-  <si>
-    <t>Samsung Electronics (Preferred)</t>
-  </si>
-  <si>
-    <t>Shinhan Financial Group</t>
-  </si>
-  <si>
-    <t>024110</t>
-  </si>
-  <si>
-    <t>기업은행</t>
-  </si>
-  <si>
-    <t>Industrial Bank of Korea</t>
-  </si>
-  <si>
-    <t>323410</t>
-  </si>
-  <si>
-    <t>카카오뱅크</t>
-  </si>
-  <si>
-    <t>KakaoBank</t>
-  </si>
-  <si>
-    <t>316140</t>
-  </si>
-  <si>
-    <t>우리금융지주</t>
-  </si>
-  <si>
-    <t>Woori Financial Group</t>
-  </si>
-  <si>
-    <t>112040</t>
-  </si>
-  <si>
-    <t>위메이드</t>
-  </si>
-  <si>
-    <t>Wemade</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> KOSDAQ</t>
-  </si>
-  <si>
-    <t>067160</t>
-  </si>
-  <si>
-    <t>소프트캠프</t>
-  </si>
-  <si>
-    <t>Softcamp</t>
-  </si>
-  <si>
-    <t>225570</t>
-  </si>
-  <si>
-    <t>넥슨게임즈</t>
-  </si>
-  <si>
-    <t>Nexon Games</t>
-  </si>
-  <si>
-    <t>263750</t>
   </si>
   <si>
     <t>067080</t>
@@ -1228,7 +1231,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1264,6 +1267,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -3158,7 +3164,7 @@
       <c r="A43" t="s" s="9">
         <v>129</v>
       </c>
-      <c r="B43" t="s" s="10">
+      <c r="B43" t="s" s="12">
         <v>130</v>
       </c>
       <c r="C43" t="s" s="11">
@@ -3591,7 +3597,7 @@
         <v>196</v>
       </c>
       <c r="B67" t="s" s="10">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="C67" t="s" s="11">
         <v>167</v>
@@ -3606,13 +3612,13 @@
     </row>
     <row r="68" ht="13.5" customHeight="1">
       <c r="A68" t="s" s="9">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B68" t="s" s="10">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C68" t="s" s="11">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D68" t="s" s="7">
         <v>8</v>
@@ -3624,13 +3630,13 @@
     </row>
     <row r="69" ht="13.5" customHeight="1">
       <c r="A69" t="s" s="9">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B69" t="s" s="10">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C69" t="s" s="11">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D69" t="s" s="7">
         <v>8</v>
@@ -3642,16 +3648,16 @@
     </row>
     <row r="70" ht="13.5" customHeight="1">
       <c r="A70" t="s" s="9">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B70" t="s" s="10">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C70" t="s" s="11">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E70" t="s" s="7">
         <v>9</v>
@@ -3660,16 +3666,16 @@
     </row>
     <row r="71" ht="13.5" customHeight="1">
       <c r="A71" t="s" s="9">
+        <v>207</v>
+      </c>
+      <c r="B71" t="s" s="10">
+        <v>208</v>
+      </c>
+      <c r="C71" t="s" s="11">
+        <v>208</v>
+      </c>
+      <c r="D71" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="B71" t="s" s="10">
-        <v>207</v>
-      </c>
-      <c r="C71" t="s" s="11">
-        <v>207</v>
-      </c>
-      <c r="D71" t="s" s="2">
-        <v>205</v>
       </c>
       <c r="E71" t="s" s="2">
         <v>9</v>
@@ -3678,16 +3684,16 @@
     </row>
     <row r="72" ht="13.5" customHeight="1">
       <c r="A72" t="s" s="9">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B72" t="s" s="10">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C72" t="s" s="11">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D72" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E72" t="s" s="2">
         <v>9</v>
@@ -3696,16 +3702,16 @@
     </row>
     <row r="73" ht="13.5" customHeight="1">
       <c r="A73" t="s" s="9">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B73" t="s" s="10">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C73" t="s" s="11">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D73" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E73" t="s" s="2">
         <v>9</v>
@@ -3714,16 +3720,16 @@
     </row>
     <row r="74" ht="13.5" customHeight="1">
       <c r="A74" t="s" s="9">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B74" t="s" s="10">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C74" t="s" s="11">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D74" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E74" t="s" s="7">
         <v>9</v>
@@ -3732,16 +3738,16 @@
     </row>
     <row r="75" ht="13.5" customHeight="1">
       <c r="A75" t="s" s="9">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B75" t="s" s="10">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C75" t="s" s="11">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D75" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E75" t="s" s="7">
         <v>9</v>
@@ -3750,16 +3756,16 @@
     </row>
     <row r="76" ht="13.5" customHeight="1">
       <c r="A76" t="s" s="9">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B76" t="s" s="10">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C76" t="s" s="11">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E76" t="s" s="7">
         <v>9</v>
@@ -3768,16 +3774,16 @@
     </row>
     <row r="77" ht="13.5" customHeight="1">
       <c r="A77" t="s" s="9">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B77" t="s" s="10">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C77" t="s" s="11">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D77" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E77" t="s" s="2">
         <v>9</v>
@@ -3786,16 +3792,16 @@
     </row>
     <row r="78" ht="13.5" customHeight="1">
       <c r="A78" t="s" s="9">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B78" t="s" s="10">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C78" t="s" s="11">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D78" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E78" t="s" s="2">
         <v>9</v>
@@ -3804,16 +3810,16 @@
     </row>
     <row r="79" ht="13.5" customHeight="1">
       <c r="A79" t="s" s="9">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B79" t="s" s="10">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C79" t="s" s="11">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D79" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E79" t="s" s="7">
         <v>9</v>
@@ -3822,16 +3828,16 @@
     </row>
     <row r="80" ht="13.5" customHeight="1">
       <c r="A80" t="s" s="9">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B80" t="s" s="10">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C80" t="s" s="11">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D80" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E80" t="s" s="2">
         <v>9</v>
@@ -3840,16 +3846,16 @@
     </row>
     <row r="81" ht="13.5" customHeight="1">
       <c r="A81" t="s" s="9">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B81" t="s" s="10">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C81" t="s" s="11">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D81" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E81" t="s" s="2">
         <v>9</v>
@@ -3858,16 +3864,16 @@
     </row>
     <row r="82" ht="13.5" customHeight="1">
       <c r="A82" t="s" s="9">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B82" t="s" s="10">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C82" t="s" s="11">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D82" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E82" t="s" s="7">
         <v>9</v>
@@ -3876,16 +3882,16 @@
     </row>
     <row r="83" ht="13.5" customHeight="1">
       <c r="A83" t="s" s="9">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B83" t="s" s="10">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C83" t="s" s="11">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D83" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E83" t="s" s="2">
         <v>9</v>
@@ -3894,16 +3900,16 @@
     </row>
     <row r="84" ht="13.5" customHeight="1">
       <c r="A84" t="s" s="9">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B84" t="s" s="10">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C84" t="s" s="11">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D84" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E84" t="s" s="7">
         <v>9</v>
@@ -3912,16 +3918,16 @@
     </row>
     <row r="85" ht="13.5" customHeight="1">
       <c r="A85" t="s" s="9">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B85" t="s" s="10">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C85" t="s" s="11">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D85" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E85" t="s" s="2">
         <v>9</v>
@@ -3930,16 +3936,16 @@
     </row>
     <row r="86" ht="13.5" customHeight="1">
       <c r="A86" t="s" s="9">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B86" t="s" s="10">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C86" t="s" s="11">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E86" t="s" s="7">
         <v>9</v>
@@ -3948,16 +3954,16 @@
     </row>
     <row r="87" ht="13.5" customHeight="1">
       <c r="A87" t="s" s="9">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B87" t="s" s="10">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C87" t="s" s="11">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E87" t="s" s="7">
         <v>9</v>
@@ -3966,16 +3972,16 @@
     </row>
     <row r="88" ht="13.5" customHeight="1">
       <c r="A88" t="s" s="9">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B88" t="s" s="10">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C88" t="s" s="11">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D88" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E88" t="s" s="2">
         <v>9</v>
@@ -3984,16 +3990,16 @@
     </row>
     <row r="89" ht="13.5" customHeight="1">
       <c r="A89" t="s" s="9">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B89" t="s" s="10">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C89" t="s" s="11">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D89" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E89" t="s" s="2">
         <v>9</v>
@@ -4002,16 +4008,16 @@
     </row>
     <row r="90" ht="13.5" customHeight="1">
       <c r="A90" t="s" s="9">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B90" t="s" s="10">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C90" t="s" s="11">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D90" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E90" t="s" s="2">
         <v>9</v>
@@ -4020,16 +4026,16 @@
     </row>
     <row r="91" ht="13.5" customHeight="1">
       <c r="A91" t="s" s="9">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B91" t="s" s="10">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C91" t="s" s="11">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E91" t="s" s="7">
         <v>9</v>
@@ -4038,16 +4044,16 @@
     </row>
     <row r="92" ht="13.5" customHeight="1">
       <c r="A92" t="s" s="9">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B92" t="s" s="10">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C92" t="s" s="11">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D92" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E92" t="s" s="2">
         <v>9</v>
@@ -4056,16 +4062,16 @@
     </row>
     <row r="93" ht="13.5" customHeight="1">
       <c r="A93" t="s" s="9">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B93" t="s" s="10">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C93" t="s" s="11">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E93" t="s" s="7">
         <v>9</v>
@@ -4074,16 +4080,16 @@
     </row>
     <row r="94" ht="13.5" customHeight="1">
       <c r="A94" t="s" s="9">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B94" t="s" s="10">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C94" t="s" s="11">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D94" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E94" t="s" s="2">
         <v>9</v>
@@ -4092,16 +4098,16 @@
     </row>
     <row r="95" ht="13.5" customHeight="1">
       <c r="A95" t="s" s="9">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B95" t="s" s="10">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C95" t="s" s="11">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D95" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E95" t="s" s="2">
         <v>9</v>
@@ -4110,16 +4116,16 @@
     </row>
     <row r="96" ht="16" customHeight="1">
       <c r="A96" t="s" s="9">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B96" t="s" s="10">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C96" t="s" s="11">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D96" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E96" t="s" s="7">
         <v>9</v>
@@ -4128,16 +4134,16 @@
     </row>
     <row r="97" ht="13.5" customHeight="1">
       <c r="A97" t="s" s="9">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B97" t="s" s="10">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C97" t="s" s="11">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D97" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E97" t="s" s="7">
         <v>9</v>
@@ -4146,16 +4152,16 @@
     </row>
     <row r="98" ht="13.5" customHeight="1">
       <c r="A98" t="s" s="9">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B98" t="s" s="10">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C98" t="s" s="11">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D98" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E98" t="s" s="2">
         <v>9</v>
@@ -4164,16 +4170,16 @@
     </row>
     <row r="99" ht="13.5" customHeight="1">
       <c r="A99" t="s" s="9">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B99" t="s" s="10">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C99" t="s" s="11">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D99" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E99" t="s" s="7">
         <v>9</v>
@@ -4182,16 +4188,16 @@
     </row>
     <row r="100" ht="13.5" customHeight="1">
       <c r="A100" t="s" s="9">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B100" t="s" s="10">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C100" t="s" s="11">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D100" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E100" t="s" s="2">
         <v>9</v>
@@ -4200,16 +4206,16 @@
     </row>
     <row r="101" ht="13.5" customHeight="1">
       <c r="A101" t="s" s="9">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B101" t="s" s="10">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C101" t="s" s="11">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D101" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E101" t="s" s="2">
         <v>9</v>
@@ -4218,16 +4224,16 @@
     </row>
     <row r="102" ht="13.55" customHeight="1">
       <c r="A102" t="s" s="9">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B102" t="s" s="10">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C102" t="s" s="11">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D102" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E102" t="s" s="7">
         <v>9</v>
@@ -4236,16 +4242,16 @@
     </row>
     <row r="103" ht="13.5" customHeight="1">
       <c r="A103" t="s" s="9">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B103" t="s" s="10">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C103" t="s" s="11">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D103" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E103" t="s" s="2">
         <v>9</v>
@@ -4254,16 +4260,16 @@
     </row>
     <row r="104" ht="13.5" customHeight="1">
       <c r="A104" t="s" s="9">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B104" t="s" s="10">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C104" t="s" s="11">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D104" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E104" t="s" s="7">
         <v>9</v>
@@ -4272,16 +4278,16 @@
     </row>
     <row r="105" ht="13.5" customHeight="1">
       <c r="A105" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B105" t="s" s="10">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C105" t="s" s="11">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D105" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E105" t="s" s="2">
         <v>9</v>
@@ -4290,16 +4296,16 @@
     </row>
     <row r="106" ht="13.5" customHeight="1">
       <c r="A106" t="s" s="9">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B106" t="s" s="10">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C106" t="s" s="11">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D106" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E106" t="s" s="7">
         <v>9</v>
@@ -4308,16 +4314,16 @@
     </row>
     <row r="107" ht="13.5" customHeight="1">
       <c r="A107" t="s" s="9">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B107" t="s" s="10">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C107" t="s" s="11">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D107" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E107" t="s" s="7">
         <v>9</v>
@@ -4326,16 +4332,16 @@
     </row>
     <row r="108" ht="13.5" customHeight="1">
       <c r="A108" t="s" s="9">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B108" t="s" s="10">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C108" t="s" s="11">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D108" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E108" t="s" s="2">
         <v>9</v>
@@ -4344,16 +4350,16 @@
     </row>
     <row r="109" ht="13.5" customHeight="1">
       <c r="A109" t="s" s="9">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B109" t="s" s="10">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C109" t="s" s="11">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D109" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E109" t="s" s="7">
         <v>9</v>
@@ -4362,16 +4368,16 @@
     </row>
     <row r="110" ht="13.5" customHeight="1">
       <c r="A110" t="s" s="9">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B110" t="s" s="10">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C110" t="s" s="11">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D110" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E110" t="s" s="2">
         <v>9</v>
@@ -4380,16 +4386,16 @@
     </row>
     <row r="111" ht="13.5" customHeight="1">
       <c r="A111" t="s" s="9">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B111" t="s" s="10">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C111" t="s" s="11">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D111" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E111" t="s" s="7">
         <v>9</v>
@@ -4398,16 +4404,16 @@
     </row>
     <row r="112" ht="13.5" customHeight="1">
       <c r="A112" t="s" s="9">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B112" t="s" s="10">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C112" t="s" s="11">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D112" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E112" t="s" s="2">
         <v>9</v>
@@ -4416,16 +4422,16 @@
     </row>
     <row r="113" ht="13.5" customHeight="1">
       <c r="A113" t="s" s="9">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B113" t="s" s="10">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C113" t="s" s="11">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D113" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E113" t="s" s="2">
         <v>9</v>
@@ -4434,16 +4440,16 @@
     </row>
     <row r="114" ht="13.5" customHeight="1">
       <c r="A114" t="s" s="9">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B114" t="s" s="10">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C114" t="s" s="11">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D114" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E114" t="s" s="7">
         <v>9</v>
@@ -4452,16 +4458,16 @@
     </row>
     <row r="115" ht="13.5" customHeight="1">
       <c r="A115" t="s" s="9">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B115" t="s" s="10">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C115" t="s" s="11">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D115" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E115" t="s" s="7">
         <v>9</v>
@@ -4470,16 +4476,16 @@
     </row>
     <row r="116" ht="13.5" customHeight="1">
       <c r="A116" t="s" s="9">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B116" t="s" s="10">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C116" t="s" s="11">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D116" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E116" t="s" s="2">
         <v>9</v>
@@ -4488,16 +4494,16 @@
     </row>
     <row r="117" ht="13.5" customHeight="1">
       <c r="A117" t="s" s="9">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B117" t="s" s="10">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C117" t="s" s="11">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D117" t="s" s="7">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E117" t="s" s="7">
         <v>9</v>
@@ -4506,16 +4512,16 @@
     </row>
     <row r="118" ht="13.5" customHeight="1">
       <c r="A118" t="s" s="9">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B118" t="s" s="10">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C118" t="s" s="11">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D118" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E118" t="s" s="2">
         <v>9</v>
@@ -4523,17 +4529,17 @@
       <c r="F118" s="3"/>
     </row>
     <row r="119" ht="13.5" customHeight="1">
-      <c r="A119" t="s" s="12">
-        <v>344</v>
-      </c>
-      <c r="B119" t="s" s="13">
+      <c r="A119" t="s" s="13">
         <v>345</v>
       </c>
-      <c r="C119" t="s" s="14">
+      <c r="B119" t="s" s="14">
         <v>346</v>
       </c>
+      <c r="C119" t="s" s="15">
+        <v>347</v>
+      </c>
       <c r="D119" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E119" t="s" s="2">
         <v>9</v>

</xml_diff>